<commit_message>
feat: Implement user authentication and authorization
</commit_message>
<xml_diff>
--- a/database/README.xlsx
+++ b/database/README.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/05288658922abfe3/桌面/EuroLink_WarehouseSystem/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="149" documentId="11_AD4D9D64A577C15A4A54186CF81E43EC5BDEDD81" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{464F419F-D7C9-45FD-B9A2-1B7FDFBA168D}"/>
+  <xr:revisionPtr revIDLastSave="150" documentId="11_AD4D9D64A577C15A4A54186CF81E43EC5BDEDD81" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8174AA2-3937-44FD-A9C1-75DCE6979B29}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,9 +48,6 @@
     <t>数据类型</t>
   </si>
   <si>
-    <t>role</t>
-  </si>
-  <si>
     <t>creation_time</t>
   </si>
   <si>
@@ -208,6 +205,9 @@
   </si>
   <si>
     <t>DEFAULT now() 操作时间</t>
+  </si>
+  <si>
+    <t>user_role</t>
   </si>
 </sst>
 </file>
@@ -547,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -575,7 +575,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -586,18 +586,18 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -605,37 +605,37 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -646,34 +646,34 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
         <v>22</v>
-      </c>
-      <c r="C12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -684,122 +684,122 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -810,73 +810,73 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>